<commit_message>
What I have so far on SQA signoff- Courses file
</commit_message>
<xml_diff>
--- a/TestFiles/coursestoschedule/SQASignOff-Courses To Schedule.xlsx
+++ b/TestFiles/coursestoschedule/SQASignOff-Courses To Schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="20115" windowHeight="7935"/>
+    <workbookView xWindow="120" yWindow="195" windowWidth="20115" windowHeight="7875"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="52">
   <si>
     <t>File Name</t>
   </si>
@@ -232,9 +232,6 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -254,6 +251,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -558,628 +558,674 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="8"/>
+      <c r="B3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="8"/>
+      <c r="B4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="8"/>
+      <c r="B5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="8"/>
+      <c r="B6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="8"/>
+      <c r="B7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="8"/>
+      <c r="B8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="B9" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="B10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="B11" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="B12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="B13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="B14" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="B15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="B16" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="B17" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="B18" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="B19" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="B20" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="B21" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="B22" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
+      <c r="B23" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="B24" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
+      <c r="B25" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="7"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
+      <c r="B26" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
+      <c r="B27" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
+      <c r="B28" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="7"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
+      <c r="B29" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
+      <c r="B30" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
+      <c r="B31" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
+      <c r="B32" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
+      <c r="B33" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
+      <c r="B34" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C35" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
+      <c r="B35" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
+      <c r="B36" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
+      <c r="B37" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
+      <c r="B38" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C39" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
+      <c r="B39" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
+      <c r="B40" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C41" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
+      <c r="B41" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C42" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
+      <c r="B42" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C43" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
+      <c r="B43" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C44" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
+      <c r="B44" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C45" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
+      <c r="B45" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B46" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46" s="9">
-        <v>41385</v>
-      </c>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
+      <c r="B46" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="8">
+        <v>41385</v>
+      </c>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>